<commit_message>
Moved census files to subdir & converted to .txt
Moved raw census .xls* files to kw_raw_Data_Field2014/censuses/
Converted each one to .txt manually
Deleted old plant-community diversity .xls (previously converted to .txt)
</commit_message>
<xml_diff>
--- a/kw_raw_Data_Field2014/KW_env_2014.xlsx
+++ b/kw_raw_Data_Field2014/KW_env_2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="670" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ALD_8Jun" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -468,6 +468,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -878,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1538,7 +1541,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1872,7 +1875,7 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D12">
@@ -1959,7 +1962,7 @@
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>1462.5430555555556</v>
       </c>
       <c r="D15">
@@ -2234,7 +2237,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2636,7 +2639,7 @@
       <c r="C13" s="6">
         <v>41818</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E13">
@@ -2806,7 +2809,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3379,7 +3382,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A1:J21"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3616,28 +3619,28 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6">
         <v>41800</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
+      <c r="D8" s="2">
+        <v>1462.5708333333334</v>
       </c>
       <c r="E8">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G8">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J8">
         <v>12</v>
@@ -3648,31 +3651,31 @@
         <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C9" s="6">
         <v>41800</v>
       </c>
       <c r="D9" s="2">
-        <v>1462.5708333333334</v>
+        <v>1462.588888888889</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>26</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9">
         <v>11</v>
       </c>
       <c r="J9">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3680,31 +3683,31 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6">
         <v>41800</v>
       </c>
       <c r="D10" s="2">
-        <v>1462.588888888889</v>
+        <v>1462.6</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I10">
         <v>11</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3712,31 +3715,31 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="6">
         <v>41800</v>
       </c>
       <c r="D11" s="2">
-        <v>1462.6</v>
+        <v>1462.6090277777778</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I11">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J11">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3744,31 +3747,31 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6">
         <v>41800</v>
       </c>
       <c r="D12" s="2">
-        <v>1462.6090277777778</v>
+        <v>1462.6222222222223</v>
       </c>
       <c r="E12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G12">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <v>13</v>
       </c>
       <c r="J12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3776,31 +3779,31 @@
         <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C13" s="6">
         <v>41800</v>
       </c>
       <c r="D13" s="2">
-        <v>1462.6222222222223</v>
+        <v>1462.6423611111111</v>
       </c>
       <c r="E13">
         <v>26</v>
       </c>
       <c r="F13">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I13">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J13">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3808,10 +3811,31 @@
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C14" s="6">
         <v>41800</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1462.6604166666666</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>29</v>
+      </c>
+      <c r="G14">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3819,31 +3843,31 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C15" s="6">
         <v>41800</v>
       </c>
       <c r="D15" s="2">
-        <v>1462.7</v>
+        <v>1462.6756944444444</v>
       </c>
       <c r="E15">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F15">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G15">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J15">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3851,31 +3875,31 @@
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C16" s="6">
         <v>41800</v>
       </c>
       <c r="D16" s="2">
-        <v>1462.7256944444443</v>
+        <v>1462.6861111111111</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G16">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H16">
         <v>12</v>
       </c>
       <c r="I16">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J16">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3883,31 +3907,31 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="6">
         <v>41800</v>
       </c>
       <c r="D17" s="2">
-        <v>1462.7145833333334</v>
+        <v>1462.7</v>
       </c>
       <c r="E17">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G17">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H17">
         <v>14</v>
       </c>
       <c r="I17">
+        <v>14</v>
+      </c>
+      <c r="J17">
         <v>13</v>
-      </c>
-      <c r="J17">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3915,31 +3939,31 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="6">
         <v>41800</v>
       </c>
       <c r="D18" s="2">
-        <v>1462.6423611111111</v>
+        <v>1462.7145833333334</v>
       </c>
       <c r="E18">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F18">
+        <v>32</v>
+      </c>
+      <c r="G18">
         <v>31</v>
-      </c>
-      <c r="G18">
-        <v>32</v>
       </c>
       <c r="H18">
         <v>14</v>
       </c>
       <c r="I18">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J18">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3947,13 +3971,13 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="6">
         <v>41800</v>
       </c>
       <c r="D19" s="2">
-        <v>1462.6604166666666</v>
+        <v>1462.7256944444443</v>
       </c>
       <c r="E19">
         <v>30</v>
@@ -3962,16 +3986,16 @@
         <v>29</v>
       </c>
       <c r="G19">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H19">
         <v>12</v>
       </c>
       <c r="I19">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J19">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3979,28 +4003,28 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C20" s="6">
         <v>41800</v>
       </c>
-      <c r="D20" s="2">
-        <v>1462.6756944444444</v>
+      <c r="D20" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="E20">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F20">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G20">
         <v>21</v>
       </c>
       <c r="H20">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I20">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J20">
         <v>12</v>
@@ -4011,34 +4035,16 @@
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6">
         <v>41800</v>
       </c>
-      <c r="D21" s="2">
-        <v>1462.6861111111111</v>
-      </c>
-      <c r="E21">
-        <v>31</v>
-      </c>
-      <c r="F21">
-        <v>34</v>
-      </c>
-      <c r="G21">
-        <v>39</v>
-      </c>
-      <c r="H21">
-        <v>12</v>
-      </c>
-      <c r="I21">
-        <v>11</v>
-      </c>
-      <c r="J21">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:J21">
+    <sortCondition ref="D1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5506,8 +5512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6412,7 +6418,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>